<commit_message>
added github and trello URLs for final project.
</commit_message>
<xml_diff>
--- a/class resources/final projec teams.xlsx
+++ b/class resources/final projec teams.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Team Name</t>
   </si>
@@ -112,6 +112,48 @@
   </si>
   <si>
     <t>Speed Daemons</t>
+  </si>
+  <si>
+    <t>https://github.com/sam-alston/cs480-DTM</t>
+  </si>
+  <si>
+    <t>https://github.com/Rivey724/MobileAppsFinalProject</t>
+  </si>
+  <si>
+    <t>Trello</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/7N4L97Pw/tactical-rpg</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/jVBOEz9f/team-snes-final-project</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/CLrzOFr5/smart-vault</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/EWzPH2WB/database-set-up-and-connection</t>
+  </si>
+  <si>
+    <t>https://github.com/leviwp48/Final-Project-Mobile-Apps</t>
+  </si>
+  <si>
+    <t>https://github.com/KalimotxoGood/SmartVault</t>
+  </si>
+  <si>
+    <t>https://github.com/JackWitherell/ProjectAndroidSampler</t>
+  </si>
+  <si>
+    <t>https://github.com/zeefree/cyberfoxgame1</t>
+  </si>
+  <si>
+    <t>https://github.com/480GameSuite/Arcade_App</t>
+  </si>
+  <si>
+    <t>https://github.com/WillemTheWalrus/Dank_Spots</t>
+  </si>
+  <si>
+    <t>https://github.com/jaredconn/Greenthumbs</t>
   </si>
 </sst>
 </file>
@@ -438,20 +480,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +506,11 @@
       <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -475,8 +520,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -486,8 +534,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -497,8 +551,14 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -508,8 +568,11 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -519,8 +582,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -530,8 +596,14 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -541,8 +613,11 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -552,8 +627,11 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -562,6 +640,12 @@
       </c>
       <c r="C10" t="s">
         <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated final projec teams.xlsx to include all trello URLs
</commit_message>
<xml_diff>
--- a/class resources/final projec teams.xlsx
+++ b/class resources/final projec teams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12651"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Team Name</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Sound manipulation app</t>
   </si>
   <si>
-    <t>Luis Garcia, Jack Witherell</t>
-  </si>
-  <si>
     <t>Cyber Fox Games</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>https://trello.com/b/CLrzOFr5/smart-vault</t>
   </si>
   <si>
-    <t>https://trello.com/b/EWzPH2WB/database-set-up-and-connection</t>
-  </si>
-  <si>
     <t>https://github.com/leviwp48/Final-Project-Mobile-Apps</t>
   </si>
   <si>
@@ -154,13 +148,34 @@
   </si>
   <si>
     <t>https://github.com/jaredconn/Greenthumbs</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/h3zbMXRF/game-development-roadmap</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/1OGyiVu6/greenthumbs</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/xdNUEP7R/dtm</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/EWzPH2WB/dankspots</t>
+  </si>
+  <si>
+    <t>Luis Garcia, Jack Witherell, Angel Ruiz</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/kvv6HuKJ/cs480-music-project</t>
+  </si>
+  <si>
+    <t>https://trello.com/b/i3VFz7hZ/android-stealth-game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +187,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,14 +217,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -483,17 +509,18 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.3046875" customWidth="1"/>
+    <col min="2" max="2" width="23.07421875" customWidth="1"/>
+    <col min="3" max="3" width="20.3046875" customWidth="1"/>
+    <col min="4" max="4" width="18.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,13 +531,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -521,10 +548,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -535,13 +565,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -552,13 +582,13 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -569,10 +599,13 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -583,10 +616,13 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -597,13 +633,13 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -611,45 +647,54 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed hyperlinks from teams file
</commit_message>
<xml_diff>
--- a/class resources/final projec teams.xlsx
+++ b/class resources/final projec teams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12651"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Team Name</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Dank Spots</t>
-  </si>
-  <si>
-    <t>Weed app</t>
   </si>
   <si>
     <t>William Doudna, Julian Lucas</t>
@@ -175,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,14 +184,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,17 +206,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,15 +499,15 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.3046875" customWidth="1"/>
-    <col min="2" max="2" width="23.07421875" customWidth="1"/>
-    <col min="3" max="3" width="20.3046875" customWidth="1"/>
-    <col min="4" max="4" width="18.15234375" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,13 +518,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -548,13 +535,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -565,13 +552,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -582,13 +569,13 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -599,13 +586,13 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -616,85 +603,82 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>